<commit_message>
refactor(translation): moved tests to separate py file
</commit_message>
<xml_diff>
--- a/utils/localisation_script/test-data/fetch-only-non-translated/out-meta/hi.xlsx
+++ b/utils/localisation_script/test-data/fetch-only-non-translated/out-meta/hi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>English copy</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PATH</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,16 +461,13 @@
           <t>(No Username)</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>dfsf</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>(No Username)</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>